<commit_message>
update excel for levels 4 and 5
</commit_message>
<xml_diff>
--- a/levelplans.xlsx
+++ b/levelplans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\segood\Code\help-your-selves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8AF4DE-6DEF-46E1-82A2-03DF6B5D2924}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8057D28-E348-45B3-AF04-5B3C2006D53B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="3" xr2:uid="{63797468-8D6C-4C71-B5DD-9A6D28273545}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="6" xr2:uid="{63797468-8D6C-4C71-B5DD-9A6D28273545}"/>
   </bookViews>
   <sheets>
     <sheet name="Level1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Level3" sheetId="4" r:id="rId3"/>
     <sheet name="Level4" sheetId="5" r:id="rId4"/>
     <sheet name="Level5" sheetId="6" r:id="rId5"/>
+    <sheet name="Level6" sheetId="7" r:id="rId6"/>
+    <sheet name="Level7" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="10">
   <si>
     <t>P</t>
   </si>
@@ -145,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -159,6 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1687,7 +1690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21EB3FF-C0E3-4AA2-B48D-54497D30DB87}">
   <dimension ref="A1:AO20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -2261,10 +2264,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106021D9-4A4C-4122-A84D-839AB8D649C6}">
-  <dimension ref="A1:AO19"/>
+  <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2275,55 +2278,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-    </row>
-    <row r="2" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="1"/>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
+        <v>28</v>
+      </c>
+      <c r="AE1">
+        <v>29</v>
+      </c>
+      <c r="AF1">
+        <v>30</v>
+      </c>
+      <c r="AG1">
+        <v>31</v>
+      </c>
+      <c r="AH1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
       <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="O2" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
       <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
       <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
       <c r="AK2" s="10" t="s">
         <v>5</v>
       </c>
@@ -2334,19 +2425,23 @@
       <c r="AO2" s="10"/>
     </row>
     <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="1"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="S3" s="5" t="s">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="P3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AG3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AH3" s="1"/>
       <c r="AK3" s="8"/>
       <c r="AL3" t="s">
         <v>1</v>
@@ -2359,21 +2454,25 @@
       </c>
     </row>
     <row r="4" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="K4" s="3"/>
-      <c r="O4" s="1"/>
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="AA4" s="3"/>
-      <c r="AE4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="5"/>
+      <c r="U4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
       <c r="AK4" s="4"/>
       <c r="AL4" t="s">
         <v>2</v>
@@ -2386,293 +2485,2128 @@
       </c>
     </row>
     <row r="5" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="L5" s="3"/>
+      <c r="P5" s="1"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="3"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AB5" s="3"/>
+      <c r="AF5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AH8" s="1"/>
+    </row>
+    <row r="9" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="L9" s="3"/>
+      <c r="O9" s="4"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="AB9" s="3"/>
+      <c r="AE9" s="4"/>
+      <c r="AH9" s="1"/>
+    </row>
+    <row r="10" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+    </row>
+    <row r="11" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AH11" s="1"/>
+    </row>
+    <row r="12" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="I12" s="6"/>
+      <c r="K12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="Y12" s="6"/>
+      <c r="AA12" s="1"/>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AH13" s="1"/>
+    </row>
+    <row r="14" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AH14" s="1"/>
+    </row>
+    <row r="15" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+    </row>
+    <row r="16" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="N16" s="4"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="AD16" s="4"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AN2:AO2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3251072D-CA19-45EA-BCA3-6C441F85A5F0}">
+  <dimension ref="A1:AO20"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL13" sqref="AL13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="38" max="38" width="18.77734375" customWidth="1"/>
+    <col min="40" max="40" width="4.44140625" customWidth="1"/>
+    <col min="41" max="41" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
+        <v>28</v>
+      </c>
+      <c r="AE1">
+        <v>29</v>
+      </c>
+      <c r="AF1">
+        <v>30</v>
+      </c>
+      <c r="AG1">
+        <v>31</v>
+      </c>
+      <c r="AH1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AK2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL2" s="10"/>
+      <c r="AN2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO2" s="10"/>
+    </row>
+    <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="1"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="1"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AG5" s="1"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="1"/>
       <c r="AK5" s="3"/>
       <c r="AL5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+    <row r="6" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
       <c r="Y6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AG6" s="1"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="1"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7">
+        <v>13</v>
+      </c>
       <c r="B7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="7"/>
       <c r="R7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="W7" s="1"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="6"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
+      <c r="Z7" s="3"/>
       <c r="AA7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AG7" s="1"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="1"/>
       <c r="AK7" s="9"/>
       <c r="AL7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8">
+        <v>12</v>
+      </c>
       <c r="B8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
       <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="AG8" s="1"/>
-    </row>
-    <row r="9" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="1"/>
+    </row>
+    <row r="9" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9">
+        <v>11</v>
+      </c>
       <c r="B9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="3"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
       <c r="R9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="3"/>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="1"/>
     </row>
     <row r="10" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
-      <c r="AG10" s="1"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="1"/>
     </row>
     <row r="11" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="H11" s="6"/>
-      <c r="J11" s="1"/>
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="X11" s="6"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
     </row>
     <row r="12" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+      <c r="A12">
+        <v>8</v>
+      </c>
       <c r="B12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
       <c r="R12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AG12" s="1"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="7"/>
+      <c r="AH12" s="1"/>
     </row>
     <row r="13" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13">
+        <v>7</v>
+      </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="Q13" s="1"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
       <c r="U13" s="7"/>
-      <c r="V13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AG13" s="1"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="1"/>
     </row>
     <row r="14" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="E14" s="7"/>
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
       <c r="U14" s="7"/>
-      <c r="V14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="1"/>
-      <c r="AG14" s="1"/>
-    </row>
-    <row r="15" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="1"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="1"/>
+    </row>
+    <row r="15" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="M15" s="4"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="AC15" s="4"/>
-      <c r="AE15" s="1"/>
-      <c r="AF15" s="1"/>
-      <c r="AG15" s="1"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="1"/>
     </row>
     <row r="16" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="G16" s="3"/>
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="Q16" s="9"/>
-      <c r="W16" s="3"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
-      <c r="AG16" s="1"/>
-    </row>
-    <row r="17" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="Q17" s="1"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AC17" s="1"/>
-      <c r="AG17" s="1"/>
-    </row>
-    <row r="18" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AC18" s="1"/>
-      <c r="AG18" s="1"/>
-    </row>
-    <row r="19" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AN2:AO2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7DBCE7-A0E3-4606-8CC3-DC1CF7D3285F}">
+  <dimension ref="A1:AO20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB27" sqref="AB27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="38" max="38" width="18.77734375" customWidth="1"/>
+    <col min="40" max="40" width="4.44140625" customWidth="1"/>
+    <col min="41" max="41" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
+        <v>28</v>
+      </c>
+      <c r="AE1">
+        <v>29</v>
+      </c>
+      <c r="AF1">
+        <v>30</v>
+      </c>
+      <c r="AG1">
+        <v>31</v>
+      </c>
+      <c r="AH1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AK2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL2" s="10"/>
+      <c r="AN2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO2" s="10"/>
+    </row>
+    <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="1"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="6"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="1"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="1"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="1"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="1"/>
+    </row>
+    <row r="9" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="1"/>
+    </row>
+    <row r="10" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="1"/>
+    </row>
+    <row r="11" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="1"/>
+    </row>
+    <row r="12" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="7"/>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="1"/>
+    </row>
+    <row r="14" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="1"/>
+    </row>
+    <row r="15" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="1"/>
+    </row>
+    <row r="16" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
       <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-      <c r="AE19" s="1"/>
-      <c r="AF19" s="1"/>
-      <c r="AG19" s="1"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
add level 7 to excel
</commit_message>
<xml_diff>
--- a/levelplans.xlsx
+++ b/levelplans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\segood\Code\help-your-selves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8057D28-E348-45B3-AF04-5B3C2006D53B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169DF3E2-EA26-4DC2-AA20-2B3A6C622CFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="6" xr2:uid="{63797468-8D6C-4C71-B5DD-9A6D28273545}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="Level5" sheetId="6" r:id="rId5"/>
     <sheet name="Level6" sheetId="7" r:id="rId6"/>
     <sheet name="Level7" sheetId="8" r:id="rId7"/>
+    <sheet name="Level8" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="10">
   <si>
     <t>P</t>
   </si>
@@ -2855,7 +2856,7 @@
   <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL13" sqref="AL13"/>
+      <selection activeCell="S3" sqref="S3:AG19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3733,7 +3734,894 @@
   <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB27" sqref="AB27"/>
+      <selection activeCell="T23" sqref="T23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="38" max="38" width="18.77734375" customWidth="1"/>
+    <col min="40" max="40" width="4.44140625" customWidth="1"/>
+    <col min="41" max="41" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
+        <v>28</v>
+      </c>
+      <c r="AE1">
+        <v>29</v>
+      </c>
+      <c r="AF1">
+        <v>30</v>
+      </c>
+      <c r="AG1">
+        <v>31</v>
+      </c>
+      <c r="AH1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AK2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL2" s="10"/>
+      <c r="AN2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO2" s="10"/>
+    </row>
+    <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="1"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="1"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="1"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="1"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+    </row>
+    <row r="9" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="1"/>
+    </row>
+    <row r="10" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="1"/>
+    </row>
+    <row r="11" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="1"/>
+    </row>
+    <row r="12" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="1"/>
+    </row>
+    <row r="14" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="1"/>
+    </row>
+    <row r="15" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="1"/>
+    </row>
+    <row r="16" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AN2:AO2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBEF5FFA-71C8-4431-A832-C1CD7074EE73}">
+  <dimension ref="A1:AO20"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Level creator can read non mirrored blocks with
</commit_message>
<xml_diff>
--- a/levelplans.xlsx
+++ b/levelplans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\segood\Code\help-your-selves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169DF3E2-EA26-4DC2-AA20-2B3A6C622CFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA43D2B0-A9D2-4B34-8B13-F71B99C0FA6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="6" xr2:uid="{63797468-8D6C-4C71-B5DD-9A6D28273545}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="7" xr2:uid="{63797468-8D6C-4C71-B5DD-9A6D28273545}"/>
   </bookViews>
   <sheets>
     <sheet name="Level1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="13">
   <si>
     <t>P</t>
   </si>
@@ -63,12 +63,21 @@
   <si>
     <t>Goal</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Not Moveable (not mirrored)</t>
+  </si>
+  <si>
+    <t>Not Moveable (mirrored)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +102,13 @@
     <font>
       <sz val="20"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -159,10 +175,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,14 +552,14 @@
       <c r="AA2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AG2" s="1"/>
-      <c r="AK2" s="10" t="s">
+      <c r="AK2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="10"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AL2" s="11"/>
+      <c r="AN2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AO2" s="10"/>
+      <c r="AO2" s="11"/>
     </row>
     <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
@@ -875,10 +894,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C58099AB-31B9-4E7B-A367-D64372D9CCE1}">
-  <dimension ref="A1:AO19"/>
+  <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -889,69 +908,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
+        <v>28</v>
+      </c>
+      <c r="AE1">
+        <v>29</v>
+      </c>
+      <c r="AF1">
+        <v>30</v>
+      </c>
+      <c r="AG1">
+        <v>31</v>
+      </c>
+      <c r="AH1">
+        <v>32</v>
+      </c>
     </row>
     <row r="2" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+      <c r="A2">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
       <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
       <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
-      <c r="AK2" s="10" t="s">
+      <c r="AH2" s="1"/>
+      <c r="AK2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="10"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AL2" s="11"/>
+      <c r="AN2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AO2" s="10"/>
+      <c r="AO2" s="11"/>
     </row>
     <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="S3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="1"/>
-      <c r="AG3" s="1"/>
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AH3" s="1"/>
       <c r="AK3" s="8"/>
       <c r="AL3" t="s">
         <v>1</v>
@@ -964,25 +1077,20 @@
       </c>
     </row>
     <row r="4" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="K4" s="8"/>
-      <c r="O4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="AA4" s="8"/>
-      <c r="AE4" s="1"/>
-      <c r="AG4" s="1"/>
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="T4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1"/>
+      <c r="AH4" s="1"/>
       <c r="AK4" s="4"/>
       <c r="AL4" t="s">
         <v>2</v>
@@ -995,279 +1103,348 @@
       </c>
     </row>
     <row r="5" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="T5" s="1"/>
+      <c r="L5" s="8"/>
+      <c r="P5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AG5" s="1"/>
+      <c r="AB5" s="8"/>
+      <c r="AF5" s="1"/>
+      <c r="AH5" s="1"/>
       <c r="AK5" s="3"/>
       <c r="AL5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="T6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="R6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AG6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AH6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7">
+        <v>13</v>
+      </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="P7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AG7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AH7" s="1"/>
       <c r="AK7" s="9"/>
       <c r="AL7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="J8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Z8" s="1"/>
       <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
     </row>
     <row r="9" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
       <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="T9" s="1"/>
+      <c r="R9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="Y9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
     </row>
     <row r="10" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="W10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
       <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AG10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AH10" s="1"/>
     </row>
     <row r="11" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="T11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
-      <c r="AG11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AH11" s="1"/>
     </row>
     <row r="12" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
+      <c r="R12" s="1"/>
       <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
     </row>
     <row r="13" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="7"/>
-      <c r="G13" s="8"/>
-      <c r="J13" s="1"/>
-      <c r="Q13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="R13" s="1"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="7"/>
-      <c r="W13" s="8"/>
-      <c r="Z13" s="1"/>
-      <c r="AG13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AH13" s="1"/>
     </row>
     <row r="14" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="1"/>
-      <c r="AG14" s="1"/>
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="7"/>
+      <c r="H14" s="8"/>
+      <c r="K14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="7"/>
+      <c r="X14" s="8"/>
+      <c r="AA14" s="1"/>
+      <c r="AH14" s="1"/>
     </row>
     <row r="15" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15">
+        <v>5</v>
+      </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="1"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="7"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AD15" s="1"/>
-      <c r="AE15" s="1"/>
-      <c r="AF15" s="1"/>
-      <c r="AG15" s="1"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="1"/>
+      <c r="AH15" s="1"/>
     </row>
     <row r="16" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="Q16" s="9"/>
-      <c r="AB16" s="1"/>
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
-    </row>
-    <row r="17" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AG17" s="1"/>
-    </row>
-    <row r="18" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="AG18" s="1"/>
-    </row>
-    <row r="19" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="R17" s="9"/>
+      <c r="AC17" s="1"/>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-      <c r="AE19" s="1"/>
-      <c r="AF19" s="1"/>
-      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1337,14 +1514,14 @@
       <c r="AA2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AG2" s="1"/>
-      <c r="AK2" s="10" t="s">
+      <c r="AK2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="10"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AL2" s="11"/>
+      <c r="AN2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AO2" s="10"/>
+      <c r="AO2" s="11"/>
     </row>
     <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
@@ -1840,14 +2017,14 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
-      <c r="AK2" s="10" t="s">
+      <c r="AK2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="10"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AL2" s="11"/>
+      <c r="AN2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AO2" s="10"/>
+      <c r="AO2" s="11"/>
     </row>
     <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3">
@@ -2416,14 +2593,14 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
-      <c r="AK2" s="10" t="s">
+      <c r="AK2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="10"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AL2" s="11"/>
+      <c r="AN2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AO2" s="10"/>
+      <c r="AO2" s="11"/>
     </row>
     <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3">
@@ -2856,12 +3033,12 @@
   <dimension ref="A1:AO20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:AG19"/>
+      <selection activeCell="AL8" sqref="AK3:AL8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="38" max="38" width="18.77734375" customWidth="1"/>
+    <col min="38" max="38" width="26.5546875" customWidth="1"/>
     <col min="40" max="40" width="4.44140625" customWidth="1"/>
     <col min="41" max="41" width="16.33203125" customWidth="1"/>
   </cols>
@@ -3004,14 +3181,14 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
-      <c r="AK2" s="10" t="s">
+      <c r="AK2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="10"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AL2" s="11"/>
+      <c r="AN2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AO2" s="10"/>
+      <c r="AO2" s="11"/>
     </row>
     <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3">
@@ -3033,7 +3210,7 @@
       <c r="M3" s="7"/>
       <c r="N3" s="6"/>
       <c r="O3" s="7"/>
-      <c r="P3" s="11"/>
+      <c r="P3" s="10"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="1"/>
       <c r="S3" s="7"/>
@@ -3050,7 +3227,7 @@
       <c r="AC3" s="7"/>
       <c r="AD3" s="6"/>
       <c r="AE3" s="7"/>
-      <c r="AF3" s="11"/>
+      <c r="AF3" s="10"/>
       <c r="AG3" s="7"/>
       <c r="AH3" s="1"/>
       <c r="AK3" s="8"/>
@@ -3117,20 +3294,42 @@
         <v>15</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="C5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="L5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="1"/>
       <c r="Y5" s="1"/>
@@ -3181,7 +3380,7 @@
       <c r="AH6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3220,9 +3419,11 @@
       <c r="AF7" s="6"/>
       <c r="AG7" s="7"/>
       <c r="AH7" s="1"/>
-      <c r="AK7" s="9"/>
+      <c r="AK7" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="AL7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3230,9 +3431,9 @@
         <v>12</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -3249,19 +3450,39 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
+      <c r="V8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="W8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="X8" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
+      <c r="AB8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF8" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="AG8" s="7"/>
       <c r="AH8" s="1"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9">
@@ -3280,7 +3501,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="11"/>
+      <c r="O9" s="10"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="1"/>
@@ -3296,7 +3517,7 @@
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
-      <c r="AE9" s="11"/>
+      <c r="AE9" s="10"/>
       <c r="AF9" s="7"/>
       <c r="AG9" s="7"/>
       <c r="AH9" s="1"/>
@@ -3361,17 +3582,39 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="8"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
+      <c r="T11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="W11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="X11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD11" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
@@ -3459,20 +3702,48 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
+      <c r="D14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="R14" s="1"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
@@ -3733,8 +4004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7DBCE7-A0E3-4606-8CC3-DC1CF7D3285F}">
   <dimension ref="A1:AO20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3882,14 +4153,14 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
-      <c r="AK2" s="10" t="s">
+      <c r="AK2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="10"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AL2" s="11"/>
+      <c r="AN2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AO2" s="10"/>
+      <c r="AO2" s="11"/>
     </row>
     <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3">
@@ -3909,7 +4180,7 @@
       <c r="M3" s="7"/>
       <c r="N3" s="6"/>
       <c r="O3" s="7"/>
-      <c r="P3" s="11"/>
+      <c r="P3" s="10"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="1"/>
       <c r="S3" s="7"/>
@@ -3925,7 +4196,7 @@
       <c r="AC3" s="7"/>
       <c r="AD3" s="6"/>
       <c r="AE3" s="7"/>
-      <c r="AF3" s="11"/>
+      <c r="AF3" s="10"/>
       <c r="AG3" s="7"/>
       <c r="AH3" s="1"/>
       <c r="AK3" s="8"/>
@@ -4432,7 +4703,7 @@
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="11"/>
+      <c r="N16" s="10"/>
       <c r="O16" s="7"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
@@ -4448,7 +4719,7 @@
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
       <c r="AC16" s="7"/>
-      <c r="AD16" s="11"/>
+      <c r="AD16" s="10"/>
       <c r="AE16" s="7"/>
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
@@ -4620,13 +4891,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBEF5FFA-71C8-4431-A832-C1CD7074EE73}">
   <dimension ref="A1:AO20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AO15" sqref="AO15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="38" max="38" width="18.77734375" customWidth="1"/>
+    <col min="38" max="38" width="26.5546875" customWidth="1"/>
     <col min="40" max="40" width="4.44140625" customWidth="1"/>
     <col min="41" max="41" width="16.33203125" customWidth="1"/>
   </cols>
@@ -4769,14 +5040,14 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
-      <c r="AK2" s="10" t="s">
+      <c r="AK2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="10"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AL2" s="11"/>
+      <c r="AN2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AO2" s="10"/>
+      <c r="AO2" s="11"/>
     </row>
     <row r="3" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3">
@@ -4796,7 +5067,7 @@
       <c r="M3" s="7"/>
       <c r="N3" s="6"/>
       <c r="O3" s="7"/>
-      <c r="P3" s="11"/>
+      <c r="P3" s="10"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="1"/>
       <c r="S3" s="7"/>
@@ -4812,7 +5083,7 @@
       <c r="AC3" s="7"/>
       <c r="AD3" s="6"/>
       <c r="AE3" s="7"/>
-      <c r="AF3" s="11"/>
+      <c r="AF3" s="10"/>
       <c r="AG3" s="7"/>
       <c r="AH3" s="1"/>
       <c r="AK3" s="8"/>
@@ -4929,7 +5200,9 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="6"/>
@@ -4959,7 +5232,7 @@
       <c r="AH6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -4985,7 +5258,9 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
       <c r="V7" s="8"/>
-      <c r="W7" s="1"/>
+      <c r="W7" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="X7" s="6"/>
       <c r="Y7" s="7"/>
       <c r="Z7" s="6"/>
@@ -4997,9 +5272,11 @@
       <c r="AF7" s="6"/>
       <c r="AG7" s="7"/>
       <c r="AH7" s="1"/>
-      <c r="AK7" s="9"/>
+      <c r="AK7" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="AL7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -5010,7 +5287,9 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="6"/>
       <c r="I8" s="7"/>
@@ -5039,6 +5318,10 @@
       <c r="AF8" s="6"/>
       <c r="AG8" s="7"/>
       <c r="AH8" s="1"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9">
@@ -5057,7 +5340,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="11"/>
+      <c r="O9" s="10"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="1"/>
@@ -5073,7 +5356,7 @@
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
-      <c r="AE9" s="11"/>
+      <c r="AE9" s="10"/>
       <c r="AF9" s="7"/>
       <c r="AG9" s="7"/>
       <c r="AH9" s="1"/>
@@ -5322,7 +5605,7 @@
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="11"/>
+      <c r="N16" s="10"/>
       <c r="O16" s="7"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
@@ -5338,7 +5621,7 @@
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
       <c r="AC16" s="7"/>
-      <c r="AD16" s="11"/>
+      <c r="AD16" s="10"/>
       <c r="AE16" s="7"/>
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>

</xml_diff>